<commit_message>
Database tables creation script+
</commit_message>
<xml_diff>
--- a/Database/Iteration 2 ERD Mapping.xlsx
+++ b/Database/Iteration 2 ERD Mapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="56">
   <si>
     <t>CarStock</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>Order</t>
-  </si>
-  <si>
     <t>ChipTuning</t>
   </si>
   <si>
@@ -140,18 +137,12 @@
     <t>CarSaleID</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
     <t>FK</t>
   </si>
   <si>
     <t>DATE</t>
   </si>
   <si>
-    <t>OrderID</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
@@ -183,6 +174,24 @@
   </si>
   <si>
     <t>RepairID</t>
+  </si>
+  <si>
+    <t>TransactionOrder</t>
+  </si>
+  <si>
+    <t>TransactionOrderID</t>
+  </si>
+  <si>
+    <t>SaleDate</t>
+  </si>
+  <si>
+    <t>RepairDate</t>
+  </si>
+  <si>
+    <t>ServiceDate</t>
+  </si>
+  <si>
+    <t>TuningDate</t>
   </si>
 </sst>
 </file>
@@ -654,7 +663,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +672,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
@@ -679,16 +688,16 @@
       <c r="C1" s="1"/>
       <c r="E1" s="9"/>
       <c r="F1" s="8" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="G1" s="1"/>
       <c r="I1" s="9"/>
       <c r="J1" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K1" s="1"/>
       <c r="O1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -705,7 +714,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>16</v>
@@ -714,7 +723,7 @@
         <v>2</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>16</v>
@@ -729,19 +738,19 @@
         <v>16</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>16</v>
@@ -764,7 +773,7 @@
       </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>21</v>
@@ -780,14 +789,14 @@
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I5" s="5"/>
       <c r="J5" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>21</v>
@@ -817,7 +826,7 @@
       <c r="G7" s="1"/>
       <c r="I7" s="9"/>
       <c r="J7" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -833,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>16</v>
@@ -842,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>16</v>
@@ -857,7 +866,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>1</v>
@@ -867,7 +876,7 @@
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>19</v>
@@ -883,10 +892,10 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="19" t="s">
@@ -906,7 +915,7 @@
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K11" s="18" t="s">
         <v>16</v>
@@ -922,7 +931,7 @@
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -938,14 +947,14 @@
         <v>2</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>16</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K13" s="1"/>
     </row>
@@ -959,7 +968,7 @@
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G14" s="15" t="s">
         <v>21</v>
@@ -968,7 +977,7 @@
         <v>2</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>16</v>
@@ -1007,14 +1016,14 @@
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>21</v>
@@ -1023,10 +1032,10 @@
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1037,7 +1046,7 @@
       <c r="C18" s="1"/>
       <c r="E18" s="9"/>
       <c r="F18" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="1"/>
       <c r="I18" s="5"/>
@@ -1053,7 +1062,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
@@ -1062,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G19" s="15" t="s">
         <v>16</v>
@@ -1071,14 +1080,14 @@
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="G20" s="15" t="s">
         <v>21</v>
@@ -1087,7 +1096,7 @@
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>19</v>
@@ -1103,23 +1112,23 @@
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G22" s="16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
@@ -1128,7 +1137,7 @@
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>17</v>

</xml_diff>